<commit_message>
Update existing headerfooter test.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/PageSetup/HeaderFooters.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/PageSetup/HeaderFooters.xlsx
@@ -373,12 +373,12 @@
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
-    <x:oddHeader>&amp;L&amp;"-,Regular"Created with ClosedXML</x:oddHeader>
-    <x:oddFooter>&amp;C&amp;"-,Regular"&amp;P&amp;"-,Regular" / &amp;"-,Regular"&amp;N&amp;R&amp;"-,Regular"&amp;Z&amp;F</x:oddFooter>
-    <x:evenHeader>&amp;L&amp;"-,Regular"Created with ClosedXML</x:evenHeader>
-    <x:evenFooter>&amp;C&amp;"-,Regular"&amp;P&amp;"-,Regular" / &amp;"-,Regular"&amp;N</x:evenFooter>
-    <x:firstHeader>&amp;L&amp;"-,Regular"Created with ClosedXML&amp;R&amp;"-,Bold"The &amp;"-,Regular"&amp;KFF0000First &amp;"-,Regular"&amp;E&amp;K0000FFColorful &amp;E&amp;"Broadway,Bold Italic"&amp;K000000Page</x:firstHeader>
-    <x:firstFooter>&amp;C&amp;"-,Regular"&amp;P&amp;"-,Regular" / &amp;"-,Regular"&amp;N</x:firstFooter>
+    <x:oddHeader>&amp;LCreated with ClosedXML</x:oddHeader>
+    <x:oddFooter>&amp;C&amp;P / &amp;N&amp;R&amp;Z&amp;F</x:oddFooter>
+    <x:evenHeader>&amp;LCreated with ClosedXML</x:evenHeader>
+    <x:evenFooter>&amp;C&amp;P / &amp;N</x:evenFooter>
+    <x:firstHeader>&amp;LCreated with ClosedXML&amp;R&amp;"-,Bold"The &amp;"-,Regular"&amp;KFF0000First &amp;"-,Regular"&amp;E&amp;K0000FFColorful &amp;E&amp;"Broadway,Bold Italic"&amp;K000000Page</x:firstHeader>
+    <x:firstFooter>&amp;C&amp;P / &amp;N</x:firstFooter>
   </x:headerFooter>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>